<commit_message>
moving to new machine
</commit_message>
<xml_diff>
--- a/output_excel_file3.xlsx
+++ b/output_excel_file3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Full Name</t>
+          <t>FULL NAMES</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -446,12 +446,17 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Day type</t>
+          <t>Holiday OT</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>total day types</t>
+          <t>Workday  O</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Restday OT</t>
         </is>
       </c>
     </row>
@@ -464,104 +469,186 @@
       <c r="B2" t="n">
         <v>17</v>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Benson              Ambaisi             </t>
+          <t xml:space="preserve">Joyce               Njogu               </t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>21</v>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ernest              Odinga              </t>
+          <t xml:space="preserve">Benson              Ambaisi             </t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
+        <v>21</v>
+      </c>
+      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D4" t="n">
+        <v>76.59999999999999</v>
+      </c>
+      <c r="E4" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nicholas            Awino               </t>
+          <t xml:space="preserve">Ernest              Odinga              </t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>19</v>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+        <v>5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Job                 Mwihia              </t>
+          <t xml:space="preserve">Nicholas            Awino               </t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>21</v>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+        <v>19</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve">James               Ommira              </t>
+          <t xml:space="preserve">Job                 Mwihia              </t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>19</v>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
+        <v>21</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Virginia            Ngure               </t>
+          <t xml:space="preserve">James               Ommira              </t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>23</v>
-      </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
+        <v>19</v>
+      </c>
+      <c r="C8" t="n">
+        <v>4</v>
+      </c>
+      <c r="D8" t="n">
+        <v>63.1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Walter              Ojero               </t>
+          <t xml:space="preserve">Virginia            Ngure               </t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>22</v>
-      </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
+        <v>23</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t xml:space="preserve">Walter              Ojero               </t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>22</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>57.72</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t xml:space="preserve">Barrack             Ogonji              </t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="B11" t="n">
         <v>19</v>
       </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
added an a new column called correction
</commit_message>
<xml_diff>
--- a/output_excel_file3.xlsx
+++ b/output_excel_file3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,15 +446,25 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Overtime 1.5</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Overtime 2.0</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Holiday OT</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Workday  O</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Restday OT</t>
         </is>
@@ -478,6 +488,12 @@
       <c r="E2" t="n">
         <v>0</v>
       </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -497,6 +513,12 @@
       <c r="E3" t="n">
         <v>0</v>
       </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -508,12 +530,18 @@
         <v>21</v>
       </c>
       <c r="C4" t="n">
+        <v>76.59999999999999</v>
+      </c>
+      <c r="D4" t="n">
+        <v>15</v>
+      </c>
+      <c r="E4" t="n">
         <v>4</v>
       </c>
-      <c r="D4" t="n">
+      <c r="F4" t="n">
         <v>76.59999999999999</v>
       </c>
-      <c r="E4" t="n">
+      <c r="G4" t="n">
         <v>11</v>
       </c>
     </row>
@@ -535,6 +563,12 @@
       <c r="E5" t="n">
         <v>0</v>
       </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -554,6 +588,12 @@
       <c r="E6" t="n">
         <v>0</v>
       </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -573,6 +613,12 @@
       <c r="E7" t="n">
         <v>0</v>
       </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -584,12 +630,18 @@
         <v>19</v>
       </c>
       <c r="C8" t="n">
+        <v>63.1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" t="n">
         <v>4</v>
       </c>
-      <c r="D8" t="n">
+      <c r="F8" t="n">
         <v>63.1</v>
       </c>
-      <c r="E8" t="n">
+      <c r="G8" t="n">
         <v>6</v>
       </c>
     </row>
@@ -611,6 +663,12 @@
       <c r="E9" t="n">
         <v>0</v>
       </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -622,12 +680,18 @@
         <v>22</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>57.72</v>
       </c>
       <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
         <v>57.72</v>
       </c>
-      <c r="E10" t="n">
+      <c r="G10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -647,6 +711,12 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>